<commit_message>
Creacion casos prueba para saldos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Orientacion</t>
   </si>
@@ -90,21 +90,9 @@
     <t>7</t>
   </si>
   <si>
-    <t>20513841</t>
-  </si>
-  <si>
-    <t>1989636238</t>
-  </si>
-  <si>
-    <t>USUARIOS41</t>
-  </si>
-  <si>
     <t>OSVPPRU10</t>
   </si>
   <si>
-    <t>OSVPPRU04</t>
-  </si>
-  <si>
     <t>854124014</t>
   </si>
   <si>
@@ -136,13 +124,34 @@
   </si>
   <si>
     <t>99999999,00000000</t>
+  </si>
+  <si>
+    <t>mensaje</t>
+  </si>
+  <si>
+    <t>Los productos están ocultos, puedes habilitarlos nuevamente en la opción "Productos/ Administrar productos propios".</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,14 +163,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Mic Shell Dlg"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -222,9 +223,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -234,20 +234,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -585,237 +593,542 @@
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="P1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="L2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="N2" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="O2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="4" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1">
-        <v>4567</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I8" s="1"/>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1234</v>
+      </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I11" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I12" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -827,7 +1140,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
+          <xm:sqref>B2:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
continuacion scripts saldos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>Orientacion</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>4676</t>
+  </si>
+  <si>
+    <t>escenario</t>
+  </si>
+  <si>
+    <t>Todos los productos</t>
   </si>
 </sst>
 </file>
@@ -572,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -594,6 +603,7 @@
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -645,6 +655,9 @@
       <c r="P1" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="Q1" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="7" t="s">
@@ -669,23 +682,17 @@
         <v>1234</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>31</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
@@ -722,7 +729,7 @@
       <c r="P3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -759,7 +766,7 @@
       <c r="P4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="7"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
@@ -796,7 +803,7 @@
       <c r="P5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
@@ -833,7 +840,7 @@
       <c r="P6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -870,7 +877,7 @@
       <c r="P7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
@@ -907,6 +914,7 @@
       <c r="P8" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="7">
@@ -939,6 +947,7 @@
       <c r="P9" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="7" t="s">
@@ -977,6 +986,7 @@
         <v>31</v>
       </c>
       <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="7" t="s">
@@ -1015,6 +1025,7 @@
         <v>31</v>
       </c>
       <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="7" t="s">
@@ -1053,6 +1064,7 @@
         <v>31</v>
       </c>
       <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="7" t="s">
@@ -1091,6 +1103,7 @@
         <v>31</v>
       </c>
       <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="7" t="s">
@@ -1129,6 +1142,7 @@
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustes a saldos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>Orientacion</t>
   </si>
@@ -154,6 +154,90 @@
   </si>
   <si>
     <t>Todos los productos</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Posee depositos y créditos</t>
+  </si>
+  <si>
+    <t>Posee créditos y fondos de inversión</t>
+  </si>
+  <si>
+    <t>Posee deposito, tarjeta de crédito y crediágil</t>
+  </si>
+  <si>
+    <t>Posee crédito, inversión virtual y tarjetas de créditos</t>
+  </si>
+  <si>
+    <t>Posee depositos, tarjetas créditos,inversiones y fondos de inversiones</t>
+  </si>
+  <si>
+    <t>Todos los productos ocultos</t>
+  </si>
+  <si>
+    <t>Cuentas ocultas</t>
+  </si>
+  <si>
+    <t>Sin inversion virtual y con fondos de inversion</t>
+  </si>
+  <si>
+    <t>Con inversion virtual y sin fondos de inversion</t>
+  </si>
+  <si>
+    <t>Sin inversion virtual y sin fondos de inversion</t>
+  </si>
+  <si>
+    <t>Sin crediagil</t>
+  </si>
+  <si>
+    <t>Sin creditos</t>
+  </si>
+  <si>
+    <t>Sin tarjetas de credito</t>
+  </si>
+  <si>
+    <t>Tarjetas credito ocultas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creditos ocultas   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inversiones virtuales y fondos de inversion ocultos </t>
+  </si>
+  <si>
+    <t>Inversión virtual oculta y fondo de invercion visible</t>
+  </si>
+  <si>
+    <t>Inversión virtual visible y fondo de invercion oculto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crediagil ocultas </t>
+  </si>
+  <si>
+    <t>Sin cuentas</t>
   </si>
 </sst>
 </file>
@@ -579,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -603,7 +687,7 @@
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -726,10 +810,10 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
-      <c r="P3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -763,10 +847,10 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
@@ -800,10 +884,10 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
@@ -837,10 +921,10 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -874,10 +958,10 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
@@ -914,7 +998,9 @@
       <c r="P8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="6"/>
+      <c r="Q8" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="7">
@@ -947,7 +1033,9 @@
       <c r="P9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="6"/>
+      <c r="Q9" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="7" t="s">
@@ -985,8 +1073,12 @@
       <c r="O10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="P10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="7" t="s">
@@ -1024,8 +1116,12 @@
       <c r="O11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
+      <c r="P11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="7" t="s">
@@ -1063,8 +1159,12 @@
       <c r="O12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
+      <c r="P12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="7" t="s">
@@ -1102,8 +1202,12 @@
       <c r="O13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
+      <c r="P13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="7" t="s">
@@ -1141,8 +1245,280 @@
         <v>30</v>
       </c>
       <c r="O14" s="7"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
+      <c r="P14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I17" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I21" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I22" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1154,7 +1530,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B14</xm:sqref>
+          <xm:sqref>B2:B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
se limpia funcionalidad saldos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Todo1\Automatizacion\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\inicio\saldosporproducto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
   <si>
     <t>Orientacion</t>
   </si>
@@ -238,6 +233,18 @@
   </si>
   <si>
     <t>Sin cuentas</t>
+  </si>
+  <si>
+    <t>USUCAYC01</t>
+  </si>
+  <si>
+    <t>1989647803</t>
+  </si>
+  <si>
+    <t>406-778030-20</t>
+  </si>
+  <si>
+    <t>Prestamo Personal Ta</t>
   </si>
 </sst>
 </file>
@@ -316,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -349,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +665,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -665,11 +675,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -681,9 +691,9 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
@@ -793,10 +803,10 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="13" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="H3" s="12">
         <v>1234</v>
@@ -805,9 +815,13 @@
         <v>1234</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="11"/>
+      <c r="K3" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="M3" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="7"/>
@@ -1037,7 +1051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="30">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -1544,7 +1558,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
divicion de data en el excel
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -1,14 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Todo1\Automatizacion\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\inicio\saldosporproducto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="Listas" sheetId="2" r:id="rId2"/>
+    <sheet name="General" sheetId="3" r:id="rId2"/>
+    <sheet name="Cuentas" sheetId="4" r:id="rId3"/>
+    <sheet name="TarjetasCredito" sheetId="5" r:id="rId4"/>
+    <sheet name="Creditos" sheetId="6" r:id="rId5"/>
+    <sheet name="Inversion" sheetId="7" r:id="rId6"/>
+    <sheet name="Crediagil" sheetId="8" r:id="rId7"/>
+    <sheet name="Listas" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="75">
   <si>
     <t>Orientacion</t>
   </si>
@@ -235,23 +246,26 @@
     <t>Sin cuentas</t>
   </si>
   <si>
-    <t>USUCAYC01</t>
-  </si>
-  <si>
-    <t>1989647803</t>
-  </si>
-  <si>
-    <t>406-778030-20</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Ta</t>
+    <t>406-701110-29,406-701110-29</t>
+  </si>
+  <si>
+    <t>registro01</t>
+  </si>
+  <si>
+    <t>*4676,</t>
+  </si>
+  <si>
+    <t>406-783340-04,406-783340-18</t>
+  </si>
+  <si>
+    <t>usuariotodo1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +277,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Mic Shell Dlg"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -356,9 +378,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -675,11 +695,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -691,9 +711,9 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
@@ -803,10 +823,10 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="13" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="H3" s="12">
         <v>1234</v>
@@ -815,13 +835,9 @@
         <v>1234</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11" t="s">
-        <v>73</v>
-      </c>
+      <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="7"/>
@@ -1051,7 +1067,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30">
+    <row r="10" spans="1:21">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -1554,11 +1570,458 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1234</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1234</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="K10" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Ajustes al archivo de data y logica de validacion
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -32,6 +32,319 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar el numero completo de la cuenta incluyendo los "-" y separar por ",". Ejemplo 406-701110-29, 406-701110-29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="56">
   <si>
@@ -194,20 +507,20 @@
     <t>registro01</t>
   </si>
   <si>
-    <t>*4676,</t>
-  </si>
-  <si>
     <t>406-783340-04,406-783340-18</t>
   </si>
   <si>
     <t>usuariotodo1</t>
+  </si>
+  <si>
+    <t>*4676</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +540,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -634,11 +961,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -653,6 +980,7 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="64.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -738,7 +1066,7 @@
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -761,7 +1089,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -771,7 +1099,7 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
@@ -796,7 +1124,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -806,7 +1134,7 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1005,6 +1333,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1021,16 +1350,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1180,6 +1511,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1196,15 +1528,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1355,6 +1688,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1371,15 +1705,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1533,6 +1868,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1549,11 +1885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:O7"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1888,9 +2224,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
@@ -1904,15 +2241,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2060,8 +2398,13 @@
     <row r="4" spans="1:17">
       <c r="A4" s="13"/>
     </row>
+    <row r="7" spans="1:17">
+      <c r="N7" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Ajustes a validacion de los diferente stipos de producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -114,7 +115,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
         </r>
       </text>
     </comment>
@@ -167,7 +168,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
         </r>
       </text>
     </comment>
@@ -219,7 +220,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
         </r>
       </text>
     </comment>
@@ -271,7 +272,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
         </r>
       </text>
     </comment>
@@ -323,7 +324,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ingresar un "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo *1234, *3456</t>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
         </r>
       </text>
     </comment>
@@ -346,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="60">
   <si>
     <t>Orientacion</t>
   </si>
@@ -514,6 +515,18 @@
   </si>
   <si>
     <t>*4676</t>
+  </si>
+  <si>
+    <t>****0175, ****0556, ****9636</t>
+  </si>
+  <si>
+    <t>29281026302</t>
+  </si>
+  <si>
+    <t>1111000314765</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -964,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -980,7 +993,7 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="64.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1101,10 +1114,18 @@
       <c r="K3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="s">
         <v>31</v>
@@ -1353,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1532,7 +1553,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1709,7 +1730,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1889,7 +1910,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2245,7 +2266,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Adicion de casos exitosos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="65">
   <si>
     <t>Orientacion</t>
   </si>
@@ -527,6 +527,21 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Visualizar crediagil</t>
+  </si>
+  <si>
+    <t>Visualizar creditos</t>
+  </si>
+  <si>
+    <t>Visualizar cuentas</t>
+  </si>
+  <si>
+    <t>Visualizar inversiones</t>
+  </si>
+  <si>
+    <t>Visualizar tarjetas credito</t>
   </si>
 </sst>
 </file>
@@ -977,7 +992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -1372,17 +1387,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1460,564 +1476,17 @@
       <c r="I2" s="11">
         <v>1234</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="6"/>
       <c r="Q2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="K4" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2043,26 +1512,26 @@
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="7" t="s">
-        <v>17</v>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>47</v>
+      <c r="Q3" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2074,7 +1543,7 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="12" t="s">
         <v>21</v>
       </c>
@@ -2087,340 +1556,29 @@
       <c r="I4" s="11">
         <v>1234</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="13"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="N7" s="14"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="P9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2433,7 +1591,1039 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="K5" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I5" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I6" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="14"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="C11" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="N8" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Ajustes para los escenarios de productos ocultos
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -430,9 +430,6 @@
     <t>crediagil</t>
   </si>
   <si>
-    <t>mensaje</t>
-  </si>
-  <si>
     <t>Los productos están ocultos, puedes habilitarlos nuevamente en la opción "Productos/ Administrar productos propios".</t>
   </si>
   <si>
@@ -542,6 +539,9 @@
   </si>
   <si>
     <t>Visualizar tarjetas credito</t>
+  </si>
+  <si>
+    <t>mensajeRespuesta</t>
   </si>
 </sst>
 </file>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1060,10 +1060,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1080,7 +1080,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1117,7 +1117,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1127,23 +1127,23 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1160,7 +1160,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1178,7 +1178,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1357,10 +1357,10 @@
         <v>7</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1448,10 +1448,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1486,7 +1486,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1528,10 +1528,10 @@
         <v>13</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1603,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1661,10 +1661,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1699,7 +1699,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1741,10 +1741,10 @@
         <v>15</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1870,10 +1870,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1908,7 +1908,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1950,10 +1950,10 @@
         <v>16</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2085,10 +2085,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2123,7 +2123,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2165,10 +2165,10 @@
         <v>17</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2210,10 +2210,10 @@
         <v>17</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2255,10 +2255,10 @@
         <v>17</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2419,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2477,10 +2477,10 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2557,10 +2557,10 @@
         <v>18</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:17">

</xml_diff>

<commit_message>
Ajustes iniciales de data
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Crediagil" sheetId="8" r:id="rId6"/>
     <sheet name="Listas" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="78">
   <si>
     <t>Orientacion</t>
   </si>
@@ -542,6 +542,45 @@
   </si>
   <si>
     <t>mensajeRespuesta</t>
+  </si>
+  <si>
+    <t>FIDUQA01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USUCTDC2 </t>
+  </si>
+  <si>
+    <t>406-762410-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUEBAENROL5 </t>
+  </si>
+  <si>
+    <t>FIDUQA03</t>
+  </si>
+  <si>
+    <t>0650000001366</t>
+  </si>
+  <si>
+    <t>USUCTDC11</t>
+  </si>
+  <si>
+    <t>****4632, ****6885, ****9658</t>
+  </si>
+  <si>
+    <t>001-003143-98, 001-003145-41, 001-003150-41, 406-714130-04, 406-734560-33, 406-734560-34, 406-734560-35, 406-734560-48, 406-734560-49, 406-734560-50, 406-734560-51, 406-734560-53, 406-734560-54, 406-734560-55, 406-734560-58, 406-134560-04, 406-181110-00</t>
+  </si>
+  <si>
+    <t>USUCFEI01</t>
+  </si>
+  <si>
+    <t>****1127, ****7618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posee mas no se sabe el codigo </t>
+  </si>
+  <si>
+    <t>36123456</t>
   </si>
 </sst>
 </file>
@@ -642,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,6 +715,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,14 +1443,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1464,11 +1520,9 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1478,7 +1532,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
@@ -1499,11 +1553,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1512,21 +1564,11 @@
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
       <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1544,12 +1586,8 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="11">
         <v>1234</v>
       </c>
@@ -1557,21 +1595,11 @@
         <v>1234</v>
       </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
         <v>49</v>
@@ -1603,13 +1631,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1677,11 +1706,9 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1692,7 +1719,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="7" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -1712,11 +1739,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1725,21 +1750,11 @@
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
       <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1757,11 +1772,9 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1769,22 +1782,14 @@
       <c r="I4" s="11">
         <v>1234</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
         <v>42</v>
@@ -1812,12 +1817,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -1886,12 +1892,8 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="11">
         <v>1234</v>
       </c>
@@ -1901,9 +1903,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
@@ -1921,12 +1921,8 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="11">
         <v>1234</v>
       </c>
@@ -1934,21 +1930,11 @@
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1966,11 +1952,9 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1978,22 +1962,14 @@
       <c r="I4" s="11">
         <v>1234</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
         <v>41</v>
@@ -2024,8 +2000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2034,6 +2010,8 @@
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2101,12 +2079,8 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="11">
         <v>1234</v>
       </c>
@@ -2117,9 +2091,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
@@ -2136,11 +2108,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -2149,21 +2119,11 @@
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
@@ -2181,12 +2141,8 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="11">
         <v>1234</v>
       </c>
@@ -2194,21 +2150,11 @@
         <v>1234</v>
       </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="6" t="s">
         <v>27</v>
       </c>
@@ -2226,12 +2172,8 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="11">
         <v>1234</v>
       </c>
@@ -2239,21 +2181,11 @@
         <v>1234</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="6" t="s">
         <v>27</v>
       </c>
@@ -2271,11 +2203,9 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F6" s="12"/>
       <c r="G6" s="8" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="H6" s="11">
         <v>1234</v>
@@ -2284,27 +2214,19 @@
         <v>1234</v>
       </c>
       <c r="J6" s="7"/>
-      <c r="K6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>17</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" ht="165">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -2314,33 +2236,31 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I7" s="11">
+      <c r="F7" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="19">
+        <v>1234</v>
+      </c>
+      <c r="I7" s="19">
         <v>1234</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>17</v>
+      <c r="K7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="16">
+        <v>12700025033</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
@@ -2357,11 +2277,9 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F8" s="12"/>
       <c r="G8" s="8" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H8" s="11">
         <v>1234</v>
@@ -2370,21 +2288,13 @@
         <v>1234</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="K8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6" t="s">
         <v>39</v>
@@ -2419,12 +2329,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -2573,11 +2485,9 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -2587,20 +2497,12 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Ajustes a todos los productos ocultos
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="71">
   <si>
     <t>Orientacion</t>
   </si>
@@ -439,21 +439,6 @@
     <t>Todos los productos</t>
   </si>
   <si>
-    <t>Posee depositos y créditos</t>
-  </si>
-  <si>
-    <t>Posee créditos y fondos de inversión</t>
-  </si>
-  <si>
-    <t>Posee deposito, tarjeta de crédito y crediágil</t>
-  </si>
-  <si>
-    <t>Posee crédito, inversión virtual y tarjetas de créditos</t>
-  </si>
-  <si>
-    <t>Posee depositos, tarjetas créditos,inversiones y fondos de inversiones</t>
-  </si>
-  <si>
     <t>Todos los productos ocultos</t>
   </si>
   <si>
@@ -505,27 +490,6 @@
     <t>registro01</t>
   </si>
   <si>
-    <t>406-783340-04,406-783340-18</t>
-  </si>
-  <si>
-    <t>usuariotodo1</t>
-  </si>
-  <si>
-    <t>*4676</t>
-  </si>
-  <si>
-    <t>****0175, ****0556, ****9636</t>
-  </si>
-  <si>
-    <t>29281026302</t>
-  </si>
-  <si>
-    <t>1111000314765</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Visualizar crediagil</t>
   </si>
   <si>
@@ -581,6 +545,21 @@
   </si>
   <si>
     <t>36123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUEBAICDCS2 </t>
+  </si>
+  <si>
+    <t>1989637719</t>
+  </si>
+  <si>
+    <t>Posee deposito, tarjeta de crédito</t>
+  </si>
+  <si>
+    <t>****7730, ****6093, ****1406</t>
+  </si>
+  <si>
+    <t>406-701110-29, 406-101110-15</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1114,7 +1093,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1130,12 +1109,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="F2" s="12"/>
       <c r="H2" s="11">
         <v>1234</v>
       </c>
@@ -1144,12 +1118,10 @@
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -1162,16 +1134,14 @@
         <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1180,24 +1150,18 @@
         <v>1234</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>52</v>
+      <c r="K3" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>58</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1209,216 +1173,30 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="11">
         <v>1234</v>
       </c>
       <c r="I4" s="11">
         <v>1234</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7" t="s">
-        <v>32</v>
+      <c r="P4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I8" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="K10" s="13"/>
+      <c r="K6" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1431,7 +1209,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
+          <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1443,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:O4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1504,7 +1282,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1522,7 +1300,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1532,7 +1310,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
@@ -1540,7 +1318,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1555,7 +1333,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1573,7 +1351,7 @@
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1587,7 +1365,9 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="H4" s="11">
         <v>1234</v>
       </c>
@@ -1596,13 +1376,15 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1690,7 +1472,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1708,7 +1490,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1719,14 +1501,14 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1741,7 +1523,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1759,7 +1541,7 @@
         <v>27</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1774,7 +1556,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1784,7 +1566,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1792,7 +1574,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1818,11 +1600,12 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
@@ -1876,7 +1659,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1908,7 +1691,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1921,8 +1704,12 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="H3" s="11">
         <v>1234</v>
       </c>
@@ -1939,7 +1726,7 @@
         <v>27</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1954,7 +1741,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1964,7 +1751,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1972,7 +1759,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1980,7 +1767,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2000,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:I7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2063,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -2095,7 +1883,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2110,7 +1898,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -2128,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2159,7 +1947,7 @@
         <v>27</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2190,7 +1978,7 @@
         <v>27</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2205,7 +1993,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="12"/>
       <c r="G6" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H6" s="11">
         <v>1234</v>
@@ -2218,12 +2006,12 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="165">
@@ -2237,10 +2025,10 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="17" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H7" s="19">
         <v>1234</v>
@@ -2250,21 +2038,21 @@
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="16">
         <v>12700025033</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2279,7 +2067,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="12"/>
       <c r="G8" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H8" s="11">
         <v>1234</v>
@@ -2289,7 +2077,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2297,7 +2085,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2389,7 +2177,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -2427,7 +2215,7 @@
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2472,7 +2260,7 @@
         <v>27</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2487,7 +2275,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -2497,7 +2285,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
@@ -2505,7 +2293,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17">

</xml_diff>

<commit_message>
Segundos ajustes de data
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="75">
   <si>
     <t>Orientacion</t>
   </si>
@@ -484,9 +484,6 @@
     <t>Sin cuentas</t>
   </si>
   <si>
-    <t>406-701110-29,406-701110-29</t>
-  </si>
-  <si>
     <t>registro01</t>
   </si>
   <si>
@@ -560,6 +557,21 @@
   </si>
   <si>
     <t>406-701110-29, 406-101110-15</t>
+  </si>
+  <si>
+    <t>406-725210-11, 406-725210-12, 406-725210-13, 406-725210-14, 406-725210-25, 406-725210-26, 406-725210-27, 406-725210-28, 406-125210-01, 406-125210-02, 406-125210-03, 406-125210-04</t>
+  </si>
+  <si>
+    <t>****7806, ****7767, ****4895, ****5950, ****6318, ****6682</t>
+  </si>
+  <si>
+    <t>Crediágil</t>
+  </si>
+  <si>
+    <t>invictus10</t>
+  </si>
+  <si>
+    <t>0935000000538, 0935000000832 , Falta CDT</t>
   </si>
 </sst>
 </file>
@@ -660,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -708,6 +720,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1025,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1093,39 +1117,50 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:17" s="20" customFormat="1" ht="120">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="12"/>
-      <c r="H2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="23">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="23">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="15">
+        <v>29281023956</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1141,7 +1176,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1151,17 +1186,17 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1221,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1282,7 +1317,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1300,7 +1335,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1310,7 +1345,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
@@ -1318,7 +1353,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1333,7 +1368,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1366,7 +1401,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1377,7 +1412,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
@@ -1472,7 +1507,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1490,7 +1525,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1501,14 +1536,14 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1523,7 +1558,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1556,7 +1591,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1566,7 +1601,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1659,7 +1694,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1691,7 +1726,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1705,10 +1740,10 @@
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1741,7 +1776,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1751,7 +1786,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1851,7 +1886,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -1883,7 +1918,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1898,7 +1933,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1993,7 +2028,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="12"/>
       <c r="G6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="11">
         <v>1234</v>
@@ -2006,7 +2041,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
@@ -2025,10 +2060,10 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="19">
         <v>1234</v>
@@ -2038,17 +2073,17 @@
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="16">
         <v>12700025033</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
@@ -2067,7 +2102,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="12"/>
       <c r="G8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="11">
         <v>1234</v>
@@ -2077,7 +2112,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2177,7 +2212,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>28</v>
@@ -2215,7 +2250,7 @@
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2275,7 +2310,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -2285,7 +2320,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>

</xml_diff>

<commit_message>
cambio de contraseñas por actualizacion de data
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
+++ b/SVP/src/test/resources/datadriven/inicio/saldosporproducto/saldosporproducto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -1049,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -1823,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2066,7 +2066,7 @@
         <v>61</v>
       </c>
       <c r="H7" s="19">
-        <v>1234</v>
+        <v>5555</v>
       </c>
       <c r="I7" s="19">
         <v>1234</v>

</xml_diff>